<commit_message>
verison 2 of the excel
</commit_message>
<xml_diff>
--- a/MoneyOnME.xlsx
+++ b/MoneyOnME.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Month</t>
   </si>
@@ -102,7 +102,10 @@
     <t>February(15-28)</t>
   </si>
   <si>
-    <t>75-25 on 70$/hr</t>
+    <t>70-30 on 70$/hr</t>
+  </si>
+  <si>
+    <t>Final</t>
   </si>
 </sst>
 </file>
@@ -137,14 +140,6 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
@@ -163,6 +158,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -186,7 +189,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -195,23 +198,270 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thick">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="3" tint="0.39991454817346722"/>
+      </left>
+      <right style="thick">
+        <color theme="3" tint="0.39991454817346722"/>
+      </right>
+      <top style="thick">
+        <color theme="3" tint="0.39994506668294322"/>
+      </top>
+      <bottom style="thick">
+        <color theme="3" tint="0.39994506668294322"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="3" tint="0.39991454817346722"/>
+      </left>
+      <right style="thick">
+        <color theme="3" tint="0.39994506668294322"/>
+      </right>
+      <top style="thick">
+        <color theme="3" tint="0.39994506668294322"/>
+      </top>
+      <bottom style="thick">
+        <color theme="3" tint="0.39994506668294322"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="6" tint="-0.24994659260841701"/>
       </left>
       <right style="thin">
         <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="6" tint="-0.24994659260841701"/>
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
@@ -220,52 +470,67 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="6" tint="-0.24994659260841701"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="-0.24994659260841701"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
       <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
@@ -279,38 +544,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="5"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="6"/>
-    <xf numFmtId="44" fontId="4" fillId="2" borderId="3" xfId="4" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="5"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="6" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="5" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="4" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="2" borderId="24" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="2" borderId="25" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="2" borderId="26" xfId="3" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Calculation" xfId="5" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="6" builtinId="23"/>
+    <cellStyle name="Calculation" xfId="4" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="5" builtinId="23"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="6" builtinId="18"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Output" xfId="4" builtinId="21"/>
+    <cellStyle name="Output" xfId="3" builtinId="21"/>
     <cellStyle name="Title" xfId="2" builtinId="15"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -603,10 +900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:N16"/>
+  <dimension ref="D1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E9"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -619,497 +916,616 @@
     <col min="7" max="7" width="11.28515625" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" customWidth="1"/>
     <col min="9" max="9" width="12.42578125" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" customWidth="1"/>
-    <col min="14" max="14" width="18" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14">
-      <c r="E1" s="5" t="s">
+    <row r="1" spans="4:15" ht="15.75" thickBot="1"/>
+    <row r="2" spans="4:15" ht="16.5" customHeight="1" thickTop="1">
+      <c r="D2" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="28">
+        <f>SUM(I6:I17)</f>
+        <v>38658</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-    </row>
-    <row r="2" spans="2:14">
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-    </row>
-    <row r="3" spans="2:14" ht="18" thickBot="1">
-      <c r="D3" s="1" t="s">
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="23"/>
+    </row>
+    <row r="3" spans="4:15" ht="15.75" customHeight="1" thickBot="1">
+      <c r="D3" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="29">
+        <f>SUM(L6:L17)</f>
+        <v>22782</v>
+      </c>
+      <c r="F3" s="16"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="23"/>
+    </row>
+    <row r="4" spans="4:15" ht="18" customHeight="1" thickTop="1" thickBot="1">
+      <c r="D4" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="27">
+        <f>SUM(M6:M17)</f>
+        <v>10240</v>
+      </c>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+    </row>
+    <row r="5" spans="4:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="D5" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E5" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F5" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G5" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H5" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I5" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J5" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K5" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L5" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M5" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="N5" s="21" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="2:14" ht="16.5" thickTop="1" thickBot="1">
-      <c r="D4" s="3" t="s">
+      <c r="O5" s="22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="4:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="D6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E6" s="20">
         <v>70000</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F6" s="7">
         <v>13</v>
       </c>
-      <c r="G4" s="8">
-        <f>(F4)*8</f>
+      <c r="G6" s="7">
+        <f>(F6)*8</f>
         <v>104</v>
       </c>
-      <c r="H4" s="9">
-        <f>G4*60</f>
+      <c r="H6" s="8">
+        <f>G6*60</f>
         <v>6240</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I6" s="8">
         <v>2915</v>
       </c>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9">
-        <f>H4-I4</f>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8">
+        <f>H6-I6</f>
         <v>3325</v>
       </c>
-      <c r="M4" s="9">
-        <f>G4*10</f>
+      <c r="M6" s="8">
+        <f>G6*10</f>
         <v>1040</v>
       </c>
-    </row>
-    <row r="5" spans="2:14" ht="16.5" thickTop="1" thickBot="1">
-      <c r="D5" s="3" t="s">
+      <c r="N6" s="8">
+        <f>(I6*15)/100</f>
+        <v>437.25</v>
+      </c>
+      <c r="O6" s="8">
+        <f>(I6-N6)</f>
+        <v>2477.75</v>
+      </c>
+    </row>
+    <row r="7" spans="4:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="D7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="8">
+      <c r="E7" s="5"/>
+      <c r="F7" s="3">
         <v>10</v>
       </c>
-      <c r="G5" s="8">
-        <f t="shared" ref="G5:G16" si="0">(F5)*8</f>
+      <c r="G7" s="3">
+        <f t="shared" ref="G7:G18" si="0">(F7)*8</f>
         <v>80</v>
       </c>
-      <c r="H5" s="9">
-        <f t="shared" ref="H5:H16" si="1">G5*60</f>
+      <c r="H7" s="4">
+        <f t="shared" ref="H7:H17" si="1">G7*60</f>
         <v>4800</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I7" s="4">
         <v>2915</v>
       </c>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9">
-        <f t="shared" ref="L5:L16" si="2">H5-I5</f>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4">
+        <f t="shared" ref="L7:L18" si="2">H7-I7</f>
         <v>1885</v>
       </c>
-      <c r="M5" s="9">
-        <f t="shared" ref="M5:M16" si="3">G5*10</f>
+      <c r="M7" s="4">
+        <f t="shared" ref="M7:M18" si="3">G7*10</f>
         <v>800</v>
       </c>
-    </row>
-    <row r="6" spans="2:14" ht="16.5" thickTop="1" thickBot="1">
-      <c r="D6" s="3" t="s">
+      <c r="N7" s="4">
+        <f t="shared" ref="N7:N18" si="4">(I7*15)/100</f>
+        <v>437.25</v>
+      </c>
+      <c r="O7" s="8">
+        <f t="shared" ref="O7:O18" si="5">(I7-N7)</f>
+        <v>2477.75</v>
+      </c>
+    </row>
+    <row r="8" spans="4:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="D8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="8">
+      <c r="E8" s="5"/>
+      <c r="F8" s="3">
         <v>10</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H8" s="4">
         <f t="shared" si="1"/>
         <v>4800</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I8" s="4">
         <v>2915</v>
       </c>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9">
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4">
         <f t="shared" si="2"/>
         <v>1885</v>
       </c>
-      <c r="M6" s="9">
+      <c r="M8" s="4">
         <f t="shared" si="3"/>
         <v>800</v>
       </c>
-    </row>
-    <row r="7" spans="2:14" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="4">
-        <f>SUM(I4:I15)</f>
-        <v>38658</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="N8" s="4">
+        <f t="shared" si="4"/>
+        <v>437.25</v>
+      </c>
+      <c r="O8" s="8">
+        <f t="shared" si="5"/>
+        <v>2477.75</v>
+      </c>
+    </row>
+    <row r="9" spans="4:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="D9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="8">
+      <c r="E9" s="5"/>
+      <c r="F9" s="3">
         <v>9</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H9" s="4">
         <f t="shared" si="1"/>
         <v>4320</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I9" s="4">
         <v>2915</v>
       </c>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9">
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4">
         <f t="shared" si="2"/>
         <v>1405</v>
       </c>
-      <c r="M7" s="9">
+      <c r="M9" s="4">
         <f t="shared" si="3"/>
         <v>720</v>
       </c>
-    </row>
-    <row r="8" spans="2:14" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="4">
-        <f>SUM(L4:L15)</f>
-        <v>22782</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="N9" s="4">
+        <f t="shared" si="4"/>
+        <v>437.25</v>
+      </c>
+      <c r="O9" s="8">
+        <f t="shared" si="5"/>
+        <v>2477.75</v>
+      </c>
+    </row>
+    <row r="10" spans="4:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="D10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="8">
+      <c r="E10" s="5"/>
+      <c r="F10" s="3">
         <v>12</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>96</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H10" s="4">
         <f t="shared" si="1"/>
         <v>5760</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I10" s="4">
         <v>2915</v>
       </c>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9">
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4">
         <f t="shared" si="2"/>
         <v>2845</v>
       </c>
-      <c r="M8" s="9">
+      <c r="M10" s="4">
         <f t="shared" si="3"/>
         <v>960</v>
       </c>
-    </row>
-    <row r="9" spans="2:14" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="4">
-        <f>SUM(M4:M15)</f>
-        <v>10240</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="N10" s="4">
+        <f t="shared" si="4"/>
+        <v>437.25</v>
+      </c>
+      <c r="O10" s="8">
+        <f t="shared" si="5"/>
+        <v>2477.75</v>
+      </c>
+    </row>
+    <row r="11" spans="4:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="D11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="8">
+      <c r="E11" s="5"/>
+      <c r="F11" s="3">
         <v>11</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>88</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H11" s="4">
         <f t="shared" si="1"/>
         <v>5280</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I11" s="4">
         <v>2915</v>
       </c>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9">
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4">
         <f t="shared" si="2"/>
         <v>2365</v>
       </c>
-      <c r="M9" s="9">
+      <c r="M11" s="4">
         <f t="shared" si="3"/>
         <v>880</v>
       </c>
-    </row>
-    <row r="10" spans="2:14" ht="16.5" thickTop="1" thickBot="1">
-      <c r="D10" s="3" t="s">
+      <c r="N11" s="4">
+        <f t="shared" si="4"/>
+        <v>437.25</v>
+      </c>
+      <c r="O11" s="8">
+        <f t="shared" si="5"/>
+        <v>2477.75</v>
+      </c>
+    </row>
+    <row r="12" spans="4:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="D12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F12" s="3">
         <v>10</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G12" s="3">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H12" s="4">
         <f t="shared" si="1"/>
         <v>4800</v>
       </c>
-      <c r="I10" s="9">
-        <f>(H10*70)/100</f>
+      <c r="I12" s="4">
+        <f t="shared" ref="I12:I18" si="6">(H12*70)/100</f>
         <v>3360</v>
       </c>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9">
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4">
         <f t="shared" si="2"/>
         <v>1440</v>
       </c>
-      <c r="M10" s="9">
+      <c r="M12" s="4">
         <f t="shared" si="3"/>
         <v>800</v>
       </c>
-    </row>
-    <row r="11" spans="2:14" ht="16.5" thickTop="1" thickBot="1">
-      <c r="D11" s="3" t="s">
+      <c r="N12" s="4">
+        <f t="shared" si="4"/>
+        <v>504</v>
+      </c>
+      <c r="O12" s="8">
+        <f t="shared" si="5"/>
+        <v>2856</v>
+      </c>
+    </row>
+    <row r="13" spans="4:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="D13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="8">
+      <c r="E13" s="5"/>
+      <c r="F13" s="3">
         <v>11</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G13" s="3">
         <f t="shared" si="0"/>
         <v>88</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H13" s="4">
         <f t="shared" si="1"/>
         <v>5280</v>
       </c>
-      <c r="I11" s="9">
-        <f>(H11*70)/100</f>
+      <c r="I13" s="4">
+        <f t="shared" si="6"/>
         <v>3696</v>
       </c>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9">
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4">
         <f t="shared" si="2"/>
         <v>1584</v>
       </c>
-      <c r="M11" s="9">
+      <c r="M13" s="4">
         <f t="shared" si="3"/>
         <v>880</v>
       </c>
-    </row>
-    <row r="12" spans="2:14" ht="16.5" thickTop="1" thickBot="1">
-      <c r="D12" s="3" t="s">
+      <c r="N13" s="4">
+        <f t="shared" si="4"/>
+        <v>554.4</v>
+      </c>
+      <c r="O13" s="8">
+        <f t="shared" si="5"/>
+        <v>3141.6</v>
+      </c>
+    </row>
+    <row r="14" spans="4:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="D14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="8">
+      <c r="E14" s="5"/>
+      <c r="F14" s="3">
         <v>10</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G14" s="3">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H14" s="4">
         <f t="shared" si="1"/>
         <v>4800</v>
       </c>
-      <c r="I12" s="9">
-        <f>(H12*70)/100</f>
+      <c r="I14" s="4">
+        <f t="shared" si="6"/>
         <v>3360</v>
       </c>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9">
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4">
         <f t="shared" si="2"/>
         <v>1440</v>
       </c>
-      <c r="M12" s="9">
+      <c r="M14" s="4">
         <f t="shared" si="3"/>
         <v>800</v>
       </c>
-    </row>
-    <row r="13" spans="2:14" ht="16.5" thickTop="1" thickBot="1">
-      <c r="D13" s="3" t="s">
+      <c r="N14" s="4">
+        <f t="shared" si="4"/>
+        <v>504</v>
+      </c>
+      <c r="O14" s="8">
+        <f t="shared" si="5"/>
+        <v>2856</v>
+      </c>
+    </row>
+    <row r="15" spans="4:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="D15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="8">
+      <c r="E15" s="5"/>
+      <c r="F15" s="3">
         <v>10</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G15" s="3">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H15" s="4">
         <f t="shared" si="1"/>
         <v>4800</v>
       </c>
-      <c r="I13" s="9">
-        <f>(H13*70)/100</f>
+      <c r="I15" s="4">
+        <f t="shared" si="6"/>
         <v>3360</v>
       </c>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9">
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4">
         <f t="shared" si="2"/>
         <v>1440</v>
       </c>
-      <c r="M13" s="9">
+      <c r="M15" s="4">
         <f t="shared" si="3"/>
         <v>800</v>
       </c>
-    </row>
-    <row r="14" spans="2:14" ht="16.5" thickTop="1" thickBot="1">
-      <c r="D14" s="3" t="s">
+      <c r="N15" s="4">
+        <f t="shared" si="4"/>
+        <v>504</v>
+      </c>
+      <c r="O15" s="8">
+        <f t="shared" si="5"/>
+        <v>2856</v>
+      </c>
+    </row>
+    <row r="16" spans="4:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="D16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="8">
+      <c r="E16" s="5"/>
+      <c r="F16" s="3">
         <v>12</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G16" s="3">
         <f t="shared" si="0"/>
         <v>96</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H16" s="4">
         <f t="shared" si="1"/>
         <v>5760</v>
       </c>
-      <c r="I14" s="9">
-        <f>(H14*70)/100</f>
+      <c r="I16" s="4">
+        <f t="shared" si="6"/>
         <v>4032</v>
       </c>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9">
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4">
         <f t="shared" si="2"/>
         <v>1728</v>
       </c>
-      <c r="M14" s="9">
+      <c r="M16" s="4">
         <f t="shared" si="3"/>
         <v>960</v>
       </c>
-    </row>
-    <row r="15" spans="2:14" ht="16.5" thickTop="1" thickBot="1">
-      <c r="D15" s="3" t="s">
+      <c r="N16" s="4">
+        <f t="shared" si="4"/>
+        <v>604.79999999999995</v>
+      </c>
+      <c r="O16" s="8">
+        <f t="shared" si="5"/>
+        <v>3427.2</v>
+      </c>
+    </row>
+    <row r="17" spans="4:15" ht="16.5" thickTop="1" thickBot="1">
+      <c r="D17" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="8">
+      <c r="E17" s="9"/>
+      <c r="F17" s="10">
         <v>10</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G17" s="10">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H17" s="11">
         <f t="shared" si="1"/>
         <v>4800</v>
       </c>
-      <c r="I15" s="9">
-        <f>(H15*70)/100</f>
+      <c r="I17" s="11">
+        <f t="shared" si="6"/>
         <v>3360</v>
       </c>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9">
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11">
         <f t="shared" si="2"/>
         <v>1440</v>
       </c>
-      <c r="M15" s="9">
+      <c r="M17" s="11">
         <f t="shared" si="3"/>
         <v>800</v>
       </c>
-    </row>
-    <row r="16" spans="2:14" ht="15.75" thickTop="1">
-      <c r="D16" s="6" t="s">
+      <c r="N17" s="11">
+        <f t="shared" si="4"/>
+        <v>504</v>
+      </c>
+      <c r="O17" s="11">
+        <f t="shared" si="5"/>
+        <v>2856</v>
+      </c>
+    </row>
+    <row r="18" spans="4:15" ht="15.75" thickTop="1">
+      <c r="D18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E18" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="8">
-        <v>9</v>
-      </c>
-      <c r="G16" s="8">
+      <c r="F18" s="7">
+        <v>10</v>
+      </c>
+      <c r="G18" s="7">
         <f t="shared" si="0"/>
-        <v>72</v>
-      </c>
-      <c r="H16" s="9">
-        <f>G16*70</f>
-        <v>5040</v>
-      </c>
-      <c r="I16" s="9">
-        <f>(H16*75)/100</f>
-        <v>3780</v>
-      </c>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9">
+        <v>80</v>
+      </c>
+      <c r="H18" s="8">
+        <f>G18*70</f>
+        <v>5600</v>
+      </c>
+      <c r="I18" s="8">
+        <f t="shared" si="6"/>
+        <v>3920</v>
+      </c>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8">
         <f t="shared" si="2"/>
-        <v>1260</v>
-      </c>
-      <c r="M16" s="9">
+        <v>1680</v>
+      </c>
+      <c r="M18" s="8">
         <f t="shared" si="3"/>
-        <v>720</v>
+        <v>800</v>
+      </c>
+      <c r="N18" s="4">
+        <f t="shared" si="4"/>
+        <v>588</v>
+      </c>
+      <c r="O18" s="8">
+        <f t="shared" si="5"/>
+        <v>3332</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="E4:E9"/>
-    <mergeCell ref="E10:E15"/>
-    <mergeCell ref="E1:K2"/>
+    <mergeCell ref="E6:E11"/>
+    <mergeCell ref="E12:E17"/>
+    <mergeCell ref="F2:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>